<commit_message>
Improved schedules tracking feature, added progress bar
</commit_message>
<xml_diff>
--- a/assets/sample_schedule_template.xlsx
+++ b/assets/sample_schedule_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Projects\nssf_policy_tracker\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E1F1CF-8322-4FFA-866B-646126C38892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A9B1EA-599E-4D9C-BB8C-9EF00D21EFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,10 +506,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B2">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C2">
         <v>2004</v>
@@ -553,10 +553,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B3">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C3">
         <v>2005</v>
@@ -600,10 +600,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B4">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C4">
         <v>2006</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B5">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C5">
         <v>2010</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B6">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -741,10 +741,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>10102339</v>
+        <v>10102345</v>
       </c>
       <c r="B7">
-        <v>12345678</v>
+        <v>12345680</v>
       </c>
       <c r="C7">
         <v>2016</v>

</xml_diff>

<commit_message>
Added PDF upload feature
</commit_message>
<xml_diff>
--- a/assets/sample_schedule_template.xlsx
+++ b/assets/sample_schedule_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Projects\nssf_policy_tracker\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A9B1EA-599E-4D9C-BB8C-9EF00D21EFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527C1A14-797A-4996-812E-3B02E8A9D285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,10 +506,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B2">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C2">
         <v>2004</v>
@@ -553,10 +553,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B3">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C3">
         <v>2005</v>
@@ -600,10 +600,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B4">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C4">
         <v>2006</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B5">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C5">
         <v>2010</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B6">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -741,10 +741,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>10102345</v>
+        <v>10102368</v>
       </c>
       <c r="B7">
-        <v>12345680</v>
+        <v>12345685</v>
       </c>
       <c r="C7">
         <v>2016</v>

</xml_diff>